<commit_message>
added in plotting_example possibility to have multiple subplots for each dataset, added another toy dataset: toy_plot_3 that shows how to create data for the new functionality
</commit_message>
<xml_diff>
--- a/refactored_simulation/datasets/toy/toy_plot_2.xlsx
+++ b/refactored_simulation/datasets/toy/toy_plot_2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Google Drive Sync\TU e\DSAI\Research Topics in Data Mining\code\MDDFairness\refactored_simulation\datasets\toy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32582F5E-A44C-44EF-A524-6AC15CB80048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72CA8A06-8D44-4F9A-8E77-77F9A3D011AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9585" yWindow="0" windowWidth="12795" windowHeight="15600" xr2:uid="{AD9E8CA7-6836-4F1C-B34F-5BB75D548E5E}"/>
+    <workbookView xWindow="-6345" yWindow="6015" windowWidth="12795" windowHeight="15600" xr2:uid="{AD9E8CA7-6836-4F1C-B34F-5BB75D548E5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="40">
   <si>
     <t>acc</t>
   </si>
@@ -79,9 +79,6 @@
     <t>.1</t>
   </si>
   <si>
-    <t>SVM</t>
-  </si>
-  <si>
     <t>deletion</t>
   </si>
   <si>
@@ -103,36 +100,9 @@
     <t>.18</t>
   </si>
   <si>
-    <t>.61</t>
-  </si>
-  <si>
-    <t>.84</t>
-  </si>
-  <si>
-    <t>.85</t>
-  </si>
-  <si>
-    <t>.70</t>
-  </si>
-  <si>
-    <t>.22</t>
-  </si>
-  <si>
-    <t>.19</t>
-  </si>
-  <si>
-    <t>.21</t>
-  </si>
-  <si>
     <t>1.0</t>
   </si>
   <si>
-    <t>.68</t>
-  </si>
-  <si>
-    <t>.11</t>
-  </si>
-  <si>
     <t>maj_acc</t>
   </si>
   <si>
@@ -152,16 +122,52 @@
   </si>
   <si>
     <t>.3</t>
+  </si>
+  <si>
+    <t>Data2_race</t>
+  </si>
+  <si>
+    <t>Data2_sex</t>
+  </si>
+  <si>
+    <t>Data3_sex</t>
+  </si>
+  <si>
+    <t>Data3_race</t>
+  </si>
+  <si>
+    <t>.25</t>
+  </si>
+  <si>
+    <t>.4</t>
+  </si>
+  <si>
+    <t>.7</t>
+  </si>
+  <si>
+    <t>.75</t>
+  </si>
+  <si>
+    <t>.80</t>
+  </si>
+  <si>
+    <t>.15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -503,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC42BEB3-6210-4A5A-8246-42DB346EB3B8}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,7 +536,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -539,10 +545,10 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -553,22 +559,22 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
       </c>
       <c r="H2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -579,7 +585,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
@@ -588,12 +594,12 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -605,15 +611,15 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -622,109 +628,121 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -735,22 +753,22 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="H12" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -761,7 +779,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>11</v>
@@ -770,15 +788,15 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
         <v>10</v>
@@ -787,15 +805,15 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -804,112 +822,416 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
         <v>20</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
       </c>
       <c r="C18" t="s">
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
       </c>
       <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" t="s">
         <v>15</v>
       </c>
-      <c r="E20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="D22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+      <c r="F22" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" t="s">
         <v>29</v>
       </c>
-      <c r="C21" t="s">
+      <c r="I22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>17</v>
       </c>
-      <c r="D21" t="s">
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C27" t="s">
         <v>15</v>
       </c>
-      <c r="E21" t="s">
-        <v>38</v>
+      <c r="D27" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F27" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" t="s">
+        <v>14</v>
+      </c>
+      <c r="H27" t="s">
+        <v>34</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" t="s">
+        <v>9</v>
+      </c>
+      <c r="E28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>7</v>
+      </c>
+      <c r="B52" t="s">
+        <v>8</v>
+      </c>
+      <c r="C52" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" t="s">
+        <v>33</v>
+      </c>
+      <c r="F52" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52" t="s">
+        <v>14</v>
+      </c>
+      <c r="H52" t="s">
+        <v>34</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" t="s">
+        <v>20</v>
+      </c>
+      <c r="C53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>17</v>
+      </c>
+      <c r="B54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" t="s">
+        <v>10</v>
+      </c>
+      <c r="D54" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>18</v>
+      </c>
+      <c r="B55" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>19</v>
+      </c>
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>16</v>
+      </c>
+      <c r="D56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>